<commit_message>
updated dataset template and readme to include contact_email field
</commit_message>
<xml_diff>
--- a/template/datasetTemplate.xlsx
+++ b/template/datasetTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="I3" authorId="0">
+    <comment ref="J3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t xml:space="preserve">time</t>
   </si>
@@ -118,6 +118,9 @@
     <t xml:space="preserve">dataset_acknowledgement</t>
   </si>
   <si>
+    <t xml:space="preserve">contact_email</t>
+  </si>
+  <si>
     <t xml:space="preserve">dataset_doi</t>
   </si>
   <si>
@@ -155,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt; the acknowledgment listed for the dataset &gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; Email address of data submitter. Note: This will be public information in the database. &lt;100 chars &gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;digital object identifier (doi) associated with the dataset - you can use https://zenodo.org/ among others to register a DOI&gt;</t>
@@ -530,7 +536,6 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1527,27 +1532,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="46.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="82.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="47.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="75.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="58.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="53.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="46.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="51.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="48.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="15" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="58.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="53.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="51.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="48.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="16" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1590,7 +1595,9 @@
       <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1604,48 +1611,51 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -1659,6 +1669,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
@@ -1669,8 +1680,8 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1688,6 +1699,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
@@ -1698,8 +1710,8 @@
       <c r="F4" s="2"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="2"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1717,6 +1729,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2733,7 +2746,7 @@
   </sheetPr>
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -2756,34 +2769,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -2807,34 +2820,34 @@
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>

</xml_diff>

<commit_message>
added cruise_name to template
</commit_message>
<xml_diff>
--- a/template/datasetTemplate.xlsx
+++ b/template/datasetTemplate.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t xml:space="preserve">time</t>
   </si>
@@ -84,6 +84,9 @@
     <t xml:space="preserve">dataset_make</t>
   </si>
   <si>
+    <t xml:space="preserve">offical_cruise_name(s)</t>
+  </si>
+  <si>
     <t xml:space="preserve">dataset_source</t>
   </si>
   <si>
@@ -121,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt; how dataset is made (fixed options= [assimilation, model, observation]) (&lt;50 chars) &gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;If applicable, list official cruise name associated with your dataset. ex. KOK1606 (enter each ref. in a separate row) (optional)&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt; name of your lab/institution (&lt;100 chars) &gt;</t>
@@ -1430,10 +1436,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1441,17 +1447,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="46.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="82.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="75.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="58.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="53.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="46.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="51.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="48.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="15" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="28" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="47.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="58.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="53.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="51.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="48.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="16" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1494,7 +1499,9 @@
       <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1508,48 +1515,51 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -1563,6 +1573,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
@@ -1592,6 +1603,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
@@ -1600,10 +1612,10 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="2"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1621,6 +1633,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2659,34 +2672,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -2710,34 +2723,34 @@
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>

</xml_diff>

<commit_message>
2020_06_25 updates to example files and template
</commit_message>
<xml_diff>
--- a/template/datasetTemplate.xlsx
+++ b/template/datasetTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -96,9 +96,6 @@
     <t xml:space="preserve">dataset_acknowledgement</t>
   </si>
   <si>
-    <t xml:space="preserve">contact_email</t>
-  </si>
-  <si>
     <t xml:space="preserve">dataset_history</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
     <t xml:space="preserve">climatology</t>
   </si>
   <si>
+    <t xml:space="preserve">cruise_names</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt; short name of your dataset (&lt;50 chars) &gt;</t>
   </si>
   <si>
@@ -138,9 +138,6 @@
     <t xml:space="preserve">&lt; the acknowledgment listed for the dataset &gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; Email address of data submitter. Note: This will be public information in the database. &lt;100 chars &gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt; any note about the dataset evolution, if applicable&gt;</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;null if not climatology, 1 climatology&gt; ↓</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List any cruise names associated with your dataset. (enter each ref. in a separate row). (optional). ↓</t>
   </si>
   <si>
     <t xml:space="preserve">var_short_name</t>
@@ -300,7 +300,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,6 +311,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1436,10 +1440,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1449,14 +1453,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="82.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="47.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="75.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="58.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="53.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="51.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="48.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="16" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="53.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="46.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="51.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="48.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="15" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="28" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1515,7 +1519,6 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -1557,7 +1560,7 @@
       <c r="M2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>42</v>
       </c>
       <c r="O2" s="2"/>
@@ -1573,7 +1576,6 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
@@ -1603,7 +1605,6 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
@@ -1613,9 +1614,9 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1633,7 +1634,6 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2649,8 +2649,8 @@
   </sheetPr>
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
removed offical_cruise_name(s) for cruise_names
</commit_message>
<xml_diff>
--- a/template/datasetTemplate.xlsx
+++ b/template/datasetTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">time</t>
   </si>
@@ -84,9 +84,6 @@
     <t xml:space="preserve">dataset_make</t>
   </si>
   <si>
-    <t xml:space="preserve">official_cruise_name(s)</t>
-  </si>
-  <si>
     <t xml:space="preserve">dataset_source</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt; how dataset is made (fixed options= [assimilation, model, observation]) (&lt;50 chars) &gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;If applicable, list official cruise name associated with your dataset. ex. KOK1606 (enter each ref. in a separate row) (optional)&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt; name of your lab/institution (&lt;100 chars) &gt;</t>
@@ -1440,10 +1434,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1451,16 +1445,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="46.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="82.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="75.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="53.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="46.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="51.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="48.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="15" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="28" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="47.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="53.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="46.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="51.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="48.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="14" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="27" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1503,9 +1497,7 @@
       <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1518,51 +1510,48 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -1575,7 +1564,6 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
@@ -1604,7 +1592,6 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
@@ -1613,9 +1600,9 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -1633,7 +1620,6 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2649,7 +2635,7 @@
   </sheetPr>
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -2672,34 +2658,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -2723,34 +2709,34 @@
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>

</xml_diff>